<commit_message>
EPPlus5Decorator.cs add: epplus render excel by template add: MergeDataRow(), PrintSectionSeparateLine()
</commit_message>
<xml_diff>
--- a/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
+++ b/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
@@ -7,20 +7,20 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="2940"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$15:$16</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Sheet2!$15:$16</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Template!$15:$16</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
   <si>
     <t>NEXT GENERATION COMPANY</t>
   </si>
@@ -127,9 +127,6 @@
     <t>{{NumOfColorways}}</t>
   </si>
   <si>
-    <t>{{NumOfItem}}</t>
-  </si>
-  <si>
     <t>{{ColorwayHitRate}}</t>
   </si>
   <si>
@@ -137,6 +134,21 @@
   </si>
   <si>
     <t>{{QRCode}}</t>
+  </si>
+  <si>
+    <t>{{NumOfItems}}</t>
+  </si>
+  <si>
+    <t>T2F</t>
+  </si>
+  <si>
+    <t>{{Office Name}} Sub Total</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>{{OfficeName}} Sub Total</t>
   </si>
 </sst>
 </file>
@@ -235,17 +247,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -253,11 +255,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -297,20 +309,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -618,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,18 +633,18 @@
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -665,16 +663,16 @@
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -755,41 +753,41 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12" t="s">
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="19" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -820,10 +818,10 @@
         <v>33</v>
       </c>
       <c r="J17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -831,10 +829,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -849,152 +847,100 @@
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14">
+        <f t="shared" ref="F21:K21" si="0">SUM(F18:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="15">
-        <f>SUM(F18:F23)</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="15">
-        <f>SUM(G18:G23)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="15">
-        <f>SUM(H18:H23)</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="15">
-        <f>SUM(I18:I23)</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="15">
-        <f>SUM(J18:J23)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="15">
-        <f>SUM(K18:K23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1003,32 +949,6 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
-      <formula>$H$17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
-      <formula>$H$17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="63" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
@@ -1039,10 +959,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,17 +976,17 @@
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1085,15 +1005,15 @@
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1170,16 +1090,16 @@
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11" t="s">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1205,7 +1125,7 @@
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1213,7 +1133,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1221,13 +1141,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1238,12 +1158,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1251,10 +1171,144 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14">
+        <f t="shared" ref="F28:K28" si="0">SUM(F25:F27)</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1263,11 +1317,40 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="H15:J15"/>
   </mergeCells>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="72" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LPrepared by Peter Pan&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="greaterThan" id="{9F4F2326-BC33-4EEA-9EDF-3B71758AD4FD}">
+            <xm:f>Template!$H$17</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="6"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H24</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed: always generate NewGuid fixed: use setTabSelected() to set default sheet
</commit_message>
<xml_diff>
--- a/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
+++ b/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>NEXT GENERATION COMPANY</t>
   </si>
@@ -79,9 +79,6 @@
 Hit Rate %</t>
   </si>
   <si>
-    <t>{{Product Team}}</t>
-  </si>
-  <si>
     <t>{{City}}</t>
   </si>
   <si>
@@ -97,15 +94,6 @@
     <t>T1F</t>
   </si>
   <si>
-    <t>{{Office Name}} Total</t>
-  </si>
-  <si>
-    <t>T2B</t>
-  </si>
-  <si>
-    <t>Office Description</t>
-  </si>
-  <si>
     <t>{{OfficeName}} Office</t>
   </si>
   <si>
@@ -140,9 +128,6 @@
   </si>
   <si>
     <t>T2F</t>
-  </si>
-  <si>
-    <t>{{Office Name}} Sub Total</t>
   </si>
   <si>
     <t>Total</t>
@@ -269,35 +254,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -618,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +588,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>0</v>
@@ -648,7 +605,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
         <v>2</v>
@@ -656,12 +613,12 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>1</v>
@@ -676,12 +633,12 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -689,7 +646,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -697,7 +654,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -705,7 +662,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -713,7 +670,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -721,12 +678,12 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -734,7 +691,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -742,12 +699,12 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -766,7 +723,7 @@
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -793,46 +750,46 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -845,10 +802,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -862,7 +819,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
@@ -877,10 +834,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -912,7 +869,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -927,11 +884,11 @@
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -950,7 +907,7 @@
     <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="63" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" orientation="portrait" errors="blank" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LPrepared by Peter Pan&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -959,10 +916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="B1:K29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,13 +929,8 @@
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="19"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -988,26 +940,8 @@
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>1</v>
-      </c>
+    <row r="4" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
@@ -1015,210 +949,56 @@
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>11</v>
-      </c>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
     </row>
-    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>17</v>
-      </c>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>19</v>
-      </c>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="2:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="7"/>
@@ -1228,13 +1008,8 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>28</v>
-      </c>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1245,10 +1020,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1260,45 +1032,19 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>39</v>
-      </c>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="16"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
-      <c r="F28" s="14">
-        <f t="shared" ref="F28:K28" si="0">SUM(F25:F27)</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1318,12 +1064,12 @@
     <mergeCell ref="H15:J15"/>
   </mergeCells>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1358,7 +1104,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
fixed: get sheet1 and set as default selected
</commit_message>
<xml_diff>
--- a/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
+++ b/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
@@ -576,7 +576,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +919,7 @@
   <dimension ref="B1:K29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add: auto fit column example
</commit_message>
<xml_diff>
--- a/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
+++ b/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
@@ -106,9 +106,6 @@
     <t>{{NumOfDesign}}</t>
   </si>
   <si>
-    <t>{{NumOfDesignContracted}}</t>
-  </si>
-  <si>
     <t>{{DesignHitRate}}</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>{{OfficeName}} Sub Total</t>
+  </si>
+  <si>
+    <t>{{NumOfDesignContracted}</t>
   </si>
 </sst>
 </file>
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -241,6 +241,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,6 +254,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,7 +584,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,18 +598,18 @@
       <c r="A1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -620,16 +628,16 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -685,17 +693,35 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="22" t="s">
         <v>8</v>
       </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="22" t="s">
         <v>9</v>
       </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -710,16 +736,16 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18" t="s">
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -748,37 +774,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="17" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="J17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="23" t="s">
         <v>29</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -786,10 +812,10 @@
         <v>21</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -837,7 +863,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -884,11 +910,11 @@
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -900,11 +926,13 @@
       <c r="K23" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="B13:K13"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="63" orientation="portrait" errors="blank" r:id="rId1"/>
@@ -930,24 +958,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="4" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
@@ -956,12 +984,12 @@
       <c r="B13" s="1"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>

</xml_diff>

<commit_message>
remove some unused code in JasperReport program add: url with the inserted image
</commit_message>
<xml_diff>
--- a/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
+++ b/SolutionRoot/EPPlus5/ReportTemplate/HitRateReport5/HitRateReport5Template.xlsx
@@ -133,7 +133,7 @@
     <t>{{OfficeName}} Sub Total</t>
   </si>
   <si>
-    <t>{{NumOfDesignContracted}</t>
+    <t>{{NumOfDesignContracted}}</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -215,11 +215,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -245,6 +254,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -257,7 +267,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,18 +610,18 @@
       <c r="A1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -628,16 +640,16 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -693,35 +705,35 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -736,16 +748,16 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20" t="s">
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -791,7 +803,7 @@
       <c r="F17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H17" s="7" t="s">
@@ -803,7 +815,7 @@
       <c r="J17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -858,42 +870,42 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14">
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="25">
         <f t="shared" ref="F21:K21" si="0">SUM(F18:F20)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -958,24 +970,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="4" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
@@ -984,12 +996,12 @@
       <c r="B13" s="1"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>

</xml_diff>